<commit_message>
add manifold calculation and remove in_temp
</commit_message>
<xml_diff>
--- a/kty81-110.xlsx
+++ b/kty81-110.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\Documents\AVRStudioFiles\CAN_MFA\can-mfa\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="293" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="293" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="kty110" sheetId="1" r:id="rId1"/>
     <sheet name="kty-220" sheetId="2" r:id="rId2"/>
+    <sheet name="manifold" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="90">
   <si>
     <t>c</t>
   </si>
@@ -257,14 +253,48 @@
   </si>
   <si>
     <t>Vin</t>
+  </si>
+  <si>
+    <t>VS</t>
+  </si>
+  <si>
+    <t>MPX4250</t>
+  </si>
+  <si>
+    <t>Voffs</t>
+  </si>
+  <si>
+    <t>P=(Vout* ADC-Voffs)/(VS*0,00369)</t>
+  </si>
+  <si>
+    <t>ADC</t>
+  </si>
+  <si>
+    <t>Vadc</t>
+  </si>
+  <si>
+    <t>Vref</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>P_int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -299,7 +329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -312,6 +342,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -333,7 +364,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -370,7 +401,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -467,7 +498,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -658,11 +689,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="490113016"/>
-        <c:axId val="490107528"/>
+        <c:axId val="43641856"/>
+        <c:axId val="47232512"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="490113016"/>
+        <c:axId val="43641856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -713,15 +744,15 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490107528"/>
+        <c:crossAx val="47232512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="490107528"/>
+        <c:axId val="47232512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,10 +806,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490113016"/>
+        <c:crossAx val="43641856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -816,7 +847,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -846,7 +877,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -860,7 +891,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -897,7 +928,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -989,7 +1020,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="de-DE"/>
+                  <a:endParaRPr lang="en-US"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -1166,11 +1197,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="490103216"/>
-        <c:axId val="490103608"/>
+        <c:axId val="44894080"/>
+        <c:axId val="44895616"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="490103216"/>
+        <c:axId val="44894080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,15 +1252,15 @@
                 <a:cs typeface="Calibri"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490103608"/>
+        <c:crossAx val="44895616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="490103608"/>
+        <c:axId val="44895616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1283,10 +1314,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="490103216"/>
+        <c:crossAx val="44894080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1323,7 +1354,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1748,7 +1779,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1758,13 +1789,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S42"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1805,7 +1836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-55</v>
       </c>
@@ -1852,7 +1883,7 @@
         <v>2.5600671649778726E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-50</v>
       </c>
@@ -1899,7 +1930,7 @@
         <v>1.6702248831775676E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-40</v>
       </c>
@@ -1946,7 +1977,7 @@
         <v>4.3483555908954584E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-30</v>
       </c>
@@ -1993,7 +2024,7 @@
         <v>3.2367844626168464E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-20</v>
       </c>
@@ -2040,7 +2071,7 @@
         <v>6.3669711929967399E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-10</v>
       </c>
@@ -2087,7 +2118,7 @@
         <v>0.14549554869186068</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -2134,7 +2165,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10</v>
       </c>
@@ -2181,7 +2212,7 @@
         <v>0.1297552724000571</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
@@ -2228,7 +2259,7 @@
         <v>5.1942629159818843E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>25</v>
       </c>
@@ -2275,7 +2306,7 @@
         <v>3.1912347560975857E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>30</v>
       </c>
@@ -2322,7 +2353,7 @@
         <v>2.2213080752211786E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>40</v>
       </c>
@@ -2369,7 +2400,7 @@
         <v>5.4954459541466608E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>50</v>
       </c>
@@ -2416,7 +2447,7 @@
         <v>2.8955820071868742E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>60</v>
       </c>
@@ -2463,7 +2494,7 @@
         <v>1.0620786032363109E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>70</v>
       </c>
@@ -2510,7 +2541,7 @@
         <v>1.263141617914962E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>80</v>
       </c>
@@ -2557,7 +2588,7 @@
         <v>1.4987076627994079E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>90</v>
       </c>
@@ -2604,7 +2635,7 @@
         <v>1.4919133771929676E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>100</v>
       </c>
@@ -2651,7 +2682,7 @@
         <v>1.4007691182347628E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>110</v>
       </c>
@@ -2698,7 +2729,7 @@
         <v>1.1474755425971818E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>120</v>
       </c>
@@ -2745,7 +2776,7 @@
         <v>7.6791979438641063E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>125</v>
       </c>
@@ -2799,7 +2830,7 @@
         <v>-12</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>130</v>
       </c>
@@ -2860,7 +2891,7 @@
         <v>-1459</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>140</v>
       </c>
@@ -2921,7 +2952,7 @@
         <v>-1471</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>150</v>
       </c>
@@ -2982,7 +3013,7 @@
         <v>-1483</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="I26">
         <v>250</v>
       </c>
@@ -3001,7 +3032,7 @@
         <v>-1495</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0.65629999999999999</v>
       </c>
@@ -3023,7 +3054,7 @@
         <v>-1508</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G28" t="s">
         <v>57</v>
       </c>
@@ -3057,7 +3088,7 @@
         <v>-1520</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -3106,7 +3137,7 @@
         <v>-1532</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -3159,7 +3190,7 @@
         <v>-1544</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -3216,7 +3247,7 @@
         <v>-1556</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>8</v>
       </c>
@@ -3273,7 +3304,7 @@
         <v>-1568</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>64</v>
       </c>
@@ -3330,7 +3361,7 @@
         <v>-1581</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>256</v>
       </c>
@@ -3387,7 +3418,7 @@
         <v>-1593</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G35">
         <v>2835</v>
       </c>
@@ -3425,7 +3456,7 @@
         <v>-1605</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G36">
         <v>2565</v>
       </c>
@@ -3456,7 +3487,7 @@
         <v>-1617</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G37">
         <v>2836</v>
       </c>
@@ -3487,7 +3518,7 @@
         <v>-1629</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G38">
         <v>2700</v>
       </c>
@@ -3518,7 +3549,7 @@
         <v>-1641</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.2">
       <c r="R39">
         <v>136</v>
       </c>
@@ -3527,7 +3558,7 @@
         <v>-1654</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.2">
       <c r="R40">
         <v>255</v>
       </c>
@@ -3536,7 +3567,7 @@
         <v>-3101</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>77</v>
       </c>
@@ -3559,13 +3590,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3603,7 +3634,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-55</v>
       </c>
@@ -3646,7 +3677,7 @@
         <v>1.9462493955512757E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-50</v>
       </c>
@@ -3689,7 +3720,7 @@
         <v>9.3815398755654651E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>-40</v>
       </c>
@@ -3732,7 +3763,7 @@
         <v>1.2659099213530034E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>-30</v>
       </c>
@@ -3775,7 +3806,7 @@
         <v>3.9508264340221665E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>-20</v>
       </c>
@@ -3818,7 +3849,7 @@
         <v>7.6545020834828392E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>-10</v>
       </c>
@@ -3861,7 +3892,7 @@
         <v>0.15928869912790783</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>0</v>
       </c>
@@ -3904,7 +3935,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>10</v>
       </c>
@@ -3947,7 +3978,7 @@
         <v>0.12679193655046211</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>20</v>
       </c>
@@ -3990,7 +4021,7 @@
         <v>4.4320591888793004E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>25</v>
       </c>
@@ -4033,7 +4064,7 @@
         <v>2.5999177631579187E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>30</v>
       </c>
@@ -4076,7 +4107,7 @@
         <v>1.2992350260416667E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>40</v>
       </c>
@@ -4119,7 +4150,7 @@
         <v>3.0147399318831702E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>50</v>
       </c>
@@ -4162,7 +4193,7 @@
         <v>1.2325804735250188E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>60</v>
       </c>
@@ -4205,7 +4236,7 @@
         <v>1.8808126734628179E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>70</v>
       </c>
@@ -4248,7 +4279,7 @@
         <v>2.322901027025312E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>80</v>
       </c>
@@ -4291,7 +4322,7 @@
         <v>2.5354942908654188E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>90</v>
       </c>
@@ -4334,7 +4365,7 @@
         <v>2.5744968994344534E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>100</v>
       </c>
@@ -4377,7 +4408,7 @@
         <v>2.5230899688612283E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>110</v>
       </c>
@@ -4420,7 +4451,7 @@
         <v>2.2634548611111038E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>120</v>
       </c>
@@ -4463,7 +4494,7 @@
         <v>1.4878153165485249E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>125</v>
       </c>
@@ -4506,7 +4537,7 @@
         <v>7.8631683526011777E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>130</v>
       </c>
@@ -4549,7 +4580,7 @@
         <v>8.6870466518291774E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>140</v>
       </c>
@@ -4592,7 +4623,7 @@
         <v>2.6075081574010384E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>150</v>
       </c>
@@ -4635,12 +4666,12 @@
         <v>6.0774133350202722E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="H26">
         <v>250</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>0.67059999999999997</v>
       </c>
@@ -4655,7 +4686,7 @@
         <v>13.411999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G28" t="s">
         <v>57</v>
       </c>
@@ -4682,7 +4713,7 @@
         <v>26.823999999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -4724,7 +4755,7 @@
         <v>53.647999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>64</v>
       </c>
@@ -4770,7 +4801,7 @@
         <v>107.29599999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -4820,7 +4851,7 @@
         <v>214.59199999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>8</v>
       </c>
@@ -4870,7 +4901,7 @@
         <v>429.18399999999997</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>64</v>
       </c>
@@ -4920,7 +4951,7 @@
         <v>858.36799999999994</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>256</v>
       </c>
@@ -4970,7 +5001,7 @@
         <v>1716.7359999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G35">
         <v>2835</v>
       </c>
@@ -5001,7 +5032,7 @@
         <v>3433.4719999999998</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G36">
         <v>2565</v>
       </c>
@@ -5032,7 +5063,7 @@
         <v>6866.9439999999995</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G37">
         <v>2836</v>
       </c>
@@ -5063,7 +5094,7 @@
         <v>13733.887999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="G38">
         <v>2700</v>
       </c>
@@ -5094,7 +5125,7 @@
         <v>27467.775999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N39">
         <v>8192</v>
       </c>
@@ -5113,4 +5144,1584 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L64" sqref="L64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="5.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2">
+        <f>0.04*B1</f>
+        <v>0.2</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8">
+        <f>$B$3*E2/1023</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>(F2-$B$2)/($B$1*0.000369)</f>
+        <v>-108.40108401084011</v>
+      </c>
+      <c r="H2">
+        <f>($B$3/1023)/(5*0.00369)</f>
+        <v>0.26490978497272755</v>
+      </c>
+      <c r="I2">
+        <f>$B$2/($B$1*0.00369)</f>
+        <v>10.840108401084011</v>
+      </c>
+      <c r="J2">
+        <f>($H$2*4096*E2-$I$2*4096)/4096</f>
+        <v>-10.840108401084011</v>
+      </c>
+      <c r="K2">
+        <f>ROUNDDOWN(($H$3*E2-$I$3)/4096,0)</f>
+        <v>-108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>16</v>
+      </c>
+      <c r="F3" s="8">
+        <f t="shared" ref="F3:F66" si="0">$B$3*E3/1023</f>
+        <v>7.8201368523949169E-2</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G66" si="1">(F3-$B$2)/($B$1*0.000369)</f>
+        <v>-66.015518415203701</v>
+      </c>
+      <c r="H3">
+        <v>10850</v>
+      </c>
+      <c r="I3">
+        <v>444010</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J66" si="2">($H$2*4096*E3-$I$2*4096)/4096</f>
+        <v>-6.6015518415203704</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K66" si="3">ROUNDDOWN(($H$3*E3-$I$3)/4096,0)</f>
+        <v>-66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <v>32</v>
+      </c>
+      <c r="F4" s="8">
+        <f t="shared" si="0"/>
+        <v>0.15640273704789834</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>-23.629952819567301</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="2"/>
+        <v>-2.3629952819567297</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>-23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5">
+        <v>48</v>
+      </c>
+      <c r="F5" s="8">
+        <f t="shared" si="0"/>
+        <v>0.23460410557184752</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>18.75561277606911</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="2"/>
+        <v>1.875561277606911</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>64</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>0.31280547409579668</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>61.141178371705507</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="2"/>
+        <v>6.1141178371705518</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="E7">
+        <v>80</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>0.39100684261974583</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>103.5267439673419</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>10.352674396734193</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="3"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <f>$H$2*A8</f>
+        <v>0.52981956994545509</v>
+      </c>
+      <c r="C8">
+        <f>$I$2*A8</f>
+        <v>21.680216802168022</v>
+      </c>
+      <c r="E8">
+        <v>96</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>0.46920821114369504</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>145.91230956297832</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="2"/>
+        <v>14.591230956297833</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="3"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B19" si="4">$H$2*A9</f>
+        <v>1.0596391398909102</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:C19" si="5">$I$2*A9</f>
+        <v>43.360433604336045</v>
+      </c>
+      <c r="E9">
+        <v>112</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>0.54740957966764414</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>188.29787515861469</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="2"/>
+        <v>18.829787515861476</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="3"/>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="4"/>
+        <v>2.1192782797818204</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="5"/>
+        <v>86.72086720867209</v>
+      </c>
+      <c r="E10">
+        <v>128</v>
+      </c>
+      <c r="F10" s="8">
+        <f t="shared" si="0"/>
+        <v>0.62561094819159335</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>230.68344075425114</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="2"/>
+        <v>23.068344075425117</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="3"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="4"/>
+        <v>4.2385565595636407</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="5"/>
+        <v>173.44173441734418</v>
+      </c>
+      <c r="E11">
+        <v>144</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.70381231671554256</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>273.06900634988756</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="2"/>
+        <v>27.306900634988757</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="3"/>
+        <v>273</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>32</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="4"/>
+        <v>8.4771131191272815</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="5"/>
+        <v>346.88346883468836</v>
+      </c>
+      <c r="E12">
+        <v>160</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" si="0"/>
+        <v>0.78201368523949166</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>315.45457194552392</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="2"/>
+        <v>31.545457194552398</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="3"/>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>64</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="4"/>
+        <v>16.954226238254563</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="5"/>
+        <v>693.76693766937672</v>
+      </c>
+      <c r="E13">
+        <v>176</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="0"/>
+        <v>0.86021505376344087</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>357.84013754116029</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>35.784013754116039</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="3"/>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>128</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="4"/>
+        <v>33.908452476509126</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="5"/>
+        <v>1387.5338753387534</v>
+      </c>
+      <c r="E14">
+        <v>192</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="0"/>
+        <v>0.93841642228739008</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>400.22570313679682</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>40.02257031367968</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="3"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>256</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="4"/>
+        <v>67.816904953018252</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="5"/>
+        <v>2775.0677506775069</v>
+      </c>
+      <c r="E15">
+        <v>208</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0166177908113392</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>442.61126873243319</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="2"/>
+        <v>44.26112687324332</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>442</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>512</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="4"/>
+        <v>135.6338099060365</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="5"/>
+        <v>5550.1355013550137</v>
+      </c>
+      <c r="E16">
+        <v>224</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0948191593352883</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>484.99683432806955</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="2"/>
+        <v>48.499683432806961</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1024</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="4"/>
+        <v>271.26761981207301</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="5"/>
+        <v>11100.271002710027</v>
+      </c>
+      <c r="E17">
+        <v>240</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="0"/>
+        <v>1.1730205278592376</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>527.38239992370598</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="2"/>
+        <v>52.738239992370602</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>527</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2048</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="4"/>
+        <v>542.53523962414602</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="5"/>
+        <v>22200.542005420055</v>
+      </c>
+      <c r="E18">
+        <v>256</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="0"/>
+        <v>1.2512218963831867</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>569.7679655193424</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>56.976796551934243</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="3"/>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4096</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="4"/>
+        <v>1085.070479248292</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="5"/>
+        <v>44401.08401084011</v>
+      </c>
+      <c r="E19">
+        <v>272</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3294232649071358</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>612.1535311149787</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>61.21535311149789</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="3"/>
+        <v>612</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>288</v>
+      </c>
+      <c r="F20" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4076246334310851</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>654.53909671061524</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>65.453909671061524</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="3"/>
+        <v>654</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>304</v>
+      </c>
+      <c r="F21" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4858260019550342</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>696.92466230625166</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>69.692466230625158</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="3"/>
+        <v>696</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>320</v>
+      </c>
+      <c r="F22" s="8">
+        <f t="shared" si="0"/>
+        <v>1.5640273704789833</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>739.31022790188797</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>73.931022790188806</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="3"/>
+        <v>739</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>336</v>
+      </c>
+      <c r="F23" s="8">
+        <f t="shared" si="0"/>
+        <v>1.6422287390029326</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>781.69579349752451</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>78.169579349752453</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="3"/>
+        <v>781</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>352</v>
+      </c>
+      <c r="F24" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7204301075268817</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>824.08135909316081</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="2"/>
+        <v>82.408135909316087</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="3"/>
+        <v>824</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>368</v>
+      </c>
+      <c r="F25" s="8">
+        <f t="shared" si="0"/>
+        <v>1.7986314760508308</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>866.46692468879723</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="2"/>
+        <v>86.646692468879721</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="3"/>
+        <v>866</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>384</v>
+      </c>
+      <c r="F26" s="8">
+        <f t="shared" si="0"/>
+        <v>1.8768328445747802</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>908.85249028443366</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="2"/>
+        <v>90.885249028443369</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="3"/>
+        <v>908</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>400</v>
+      </c>
+      <c r="F27" s="8">
+        <f t="shared" si="0"/>
+        <v>1.9550342130987293</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>951.23805588007008</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>95.123805588007016</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="3"/>
+        <v>951</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>416</v>
+      </c>
+      <c r="F28" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0332355816226784</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>993.62362147570639</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>99.36236214757065</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="3"/>
+        <v>993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>432</v>
+      </c>
+      <c r="F29" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1114369501466275</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1036.0091870713427</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>103.60091870713428</v>
+      </c>
+      <c r="K29">
+        <f t="shared" si="3"/>
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>448</v>
+      </c>
+      <c r="F30" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1896383186705766</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>1078.3947526669792</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>107.83947526669793</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="3"/>
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>464</v>
+      </c>
+      <c r="F31" s="8">
+        <f t="shared" si="0"/>
+        <v>2.2678396871945261</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>1120.7803182626155</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>112.07803182626158</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="3"/>
+        <v>1120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>480</v>
+      </c>
+      <c r="F32" s="8">
+        <f t="shared" si="0"/>
+        <v>2.3460410557184752</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>1163.1658838582521</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>116.31658838582521</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="3"/>
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E33">
+        <v>496</v>
+      </c>
+      <c r="F33" s="8">
+        <f t="shared" si="0"/>
+        <v>2.4242424242424243</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>1205.5514494538884</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>120.55514494538885</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="3"/>
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>512</v>
+      </c>
+      <c r="F34" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5024437927663734</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>1247.9370150495247</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>124.79370150495249</v>
+      </c>
+      <c r="K34">
+        <f t="shared" si="3"/>
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>528</v>
+      </c>
+      <c r="F35" s="8">
+        <f t="shared" si="0"/>
+        <v>2.5806451612903225</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>1290.322580645161</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>129.03225806451613</v>
+      </c>
+      <c r="K35">
+        <f t="shared" si="3"/>
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>544</v>
+      </c>
+      <c r="F36" s="8">
+        <f t="shared" si="0"/>
+        <v>2.6588465298142716</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>1332.7081462407975</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>133.27081462407978</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="3"/>
+        <v>1332</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>560</v>
+      </c>
+      <c r="F37" s="8">
+        <f t="shared" si="0"/>
+        <v>2.7370478983382207</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>1375.0937118364338</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>137.5093711836434</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="3"/>
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>576</v>
+      </c>
+      <c r="F38" s="8">
+        <f t="shared" si="0"/>
+        <v>2.8152492668621703</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>1417.4792774320704</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>141.74792774320704</v>
+      </c>
+      <c r="K38">
+        <f t="shared" si="3"/>
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>592</v>
+      </c>
+      <c r="F39" s="8">
+        <f t="shared" si="0"/>
+        <v>2.8934506353861194</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>1459.8648430277069</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>145.98648430277069</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="3"/>
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="40" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>608</v>
+      </c>
+      <c r="F40" s="8">
+        <f t="shared" si="0"/>
+        <v>2.9716520039100685</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>1502.2504086233432</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="2"/>
+        <v>150.22504086233431</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="3"/>
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="41" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>624</v>
+      </c>
+      <c r="F41" s="8">
+        <f t="shared" si="0"/>
+        <v>3.0498533724340176</v>
+      </c>
+      <c r="G41">
+        <f t="shared" si="1"/>
+        <v>1544.6359742189795</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="2"/>
+        <v>154.46359742189796</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="3"/>
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="42" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>640</v>
+      </c>
+      <c r="F42" s="8">
+        <f t="shared" si="0"/>
+        <v>3.1280547409579667</v>
+      </c>
+      <c r="G42">
+        <f t="shared" si="1"/>
+        <v>1587.0215398146158</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="2"/>
+        <v>158.70215398146161</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="3"/>
+        <v>1586</v>
+      </c>
+    </row>
+    <row r="43" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E43">
+        <v>656</v>
+      </c>
+      <c r="F43" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2062561094819158</v>
+      </c>
+      <c r="G43">
+        <f t="shared" si="1"/>
+        <v>1629.4071054102524</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="2"/>
+        <v>162.94071054102525</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="3"/>
+        <v>1629</v>
+      </c>
+    </row>
+    <row r="44" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E44">
+        <v>672</v>
+      </c>
+      <c r="F44" s="8">
+        <f t="shared" si="0"/>
+        <v>3.2844574780058653</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="1"/>
+        <v>1671.7926710058889</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="2"/>
+        <v>167.1792671005889</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="3"/>
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="45" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E45">
+        <v>688</v>
+      </c>
+      <c r="F45" s="8">
+        <f t="shared" si="0"/>
+        <v>3.3626588465298144</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="1"/>
+        <v>1714.1782366015252</v>
+      </c>
+      <c r="J45">
+        <f t="shared" si="2"/>
+        <v>171.41782366015252</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="3"/>
+        <v>1714</v>
+      </c>
+    </row>
+    <row r="46" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E46">
+        <v>704</v>
+      </c>
+      <c r="F46" s="8">
+        <f t="shared" si="0"/>
+        <v>3.4408602150537635</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="1"/>
+        <v>1756.5638021971615</v>
+      </c>
+      <c r="J46">
+        <f t="shared" si="2"/>
+        <v>175.65638021971617</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="3"/>
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="47" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E47">
+        <v>720</v>
+      </c>
+      <c r="F47" s="8">
+        <f t="shared" si="0"/>
+        <v>3.5190615835777126</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="1"/>
+        <v>1798.9493677927981</v>
+      </c>
+      <c r="J47">
+        <f t="shared" si="2"/>
+        <v>179.89493677927982</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="3"/>
+        <v>1798</v>
+      </c>
+    </row>
+    <row r="48" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E48">
+        <v>736</v>
+      </c>
+      <c r="F48" s="8">
+        <f t="shared" si="0"/>
+        <v>3.5972629521016617</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="1"/>
+        <v>1841.3349333884344</v>
+      </c>
+      <c r="J48">
+        <f t="shared" si="2"/>
+        <v>184.13349333884344</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="3"/>
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="49" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <v>752</v>
+      </c>
+      <c r="F49" s="8">
+        <f t="shared" si="0"/>
+        <v>3.6754643206256108</v>
+      </c>
+      <c r="G49">
+        <f t="shared" si="1"/>
+        <v>1883.7204989840707</v>
+      </c>
+      <c r="J49">
+        <f t="shared" si="2"/>
+        <v>188.37204989840708</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="3"/>
+        <v>1883</v>
+      </c>
+    </row>
+    <row r="50" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E50">
+        <v>768</v>
+      </c>
+      <c r="F50" s="8">
+        <f t="shared" si="0"/>
+        <v>3.7536656891495603</v>
+      </c>
+      <c r="G50">
+        <f t="shared" si="1"/>
+        <v>1926.1060645797074</v>
+      </c>
+      <c r="J50">
+        <f t="shared" si="2"/>
+        <v>192.61060645797073</v>
+      </c>
+      <c r="K50">
+        <f t="shared" si="3"/>
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="51" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E51">
+        <v>784</v>
+      </c>
+      <c r="F51" s="8">
+        <f t="shared" si="0"/>
+        <v>3.8318670576735094</v>
+      </c>
+      <c r="G51">
+        <f t="shared" si="1"/>
+        <v>1968.4916301753437</v>
+      </c>
+      <c r="J51">
+        <f t="shared" si="2"/>
+        <v>196.84916301753438</v>
+      </c>
+      <c r="K51">
+        <f t="shared" si="3"/>
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="52" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E52">
+        <v>800</v>
+      </c>
+      <c r="F52" s="8">
+        <f t="shared" si="0"/>
+        <v>3.9100684261974585</v>
+      </c>
+      <c r="G52">
+        <f t="shared" si="1"/>
+        <v>2010.8771957709801</v>
+      </c>
+      <c r="J52">
+        <f t="shared" si="2"/>
+        <v>201.08771957709803</v>
+      </c>
+      <c r="K52">
+        <f t="shared" si="3"/>
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="53" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E53">
+        <v>816</v>
+      </c>
+      <c r="F53" s="8">
+        <f t="shared" si="0"/>
+        <v>3.9882697947214076</v>
+      </c>
+      <c r="G53">
+        <f t="shared" si="1"/>
+        <v>2053.2627613666164</v>
+      </c>
+      <c r="J53">
+        <f t="shared" si="2"/>
+        <v>205.32627613666165</v>
+      </c>
+      <c r="K53">
+        <f t="shared" si="3"/>
+        <v>2053</v>
+      </c>
+    </row>
+    <row r="54" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E54">
+        <v>832</v>
+      </c>
+      <c r="F54" s="8">
+        <f t="shared" si="0"/>
+        <v>4.0664711632453567</v>
+      </c>
+      <c r="G54">
+        <f t="shared" si="1"/>
+        <v>2095.6483269622527</v>
+      </c>
+      <c r="J54">
+        <f t="shared" si="2"/>
+        <v>209.5648326962253</v>
+      </c>
+      <c r="K54">
+        <f t="shared" si="3"/>
+        <v>2095</v>
+      </c>
+    </row>
+    <row r="55" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E55">
+        <v>848</v>
+      </c>
+      <c r="F55" s="8">
+        <f t="shared" si="0"/>
+        <v>4.1446725317693058</v>
+      </c>
+      <c r="G55">
+        <f t="shared" si="1"/>
+        <v>2138.033892557889</v>
+      </c>
+      <c r="J55">
+        <f t="shared" si="2"/>
+        <v>213.80338925578894</v>
+      </c>
+      <c r="K55">
+        <f t="shared" si="3"/>
+        <v>2137</v>
+      </c>
+    </row>
+    <row r="56" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E56">
+        <v>864</v>
+      </c>
+      <c r="F56" s="8">
+        <f t="shared" si="0"/>
+        <v>4.2228739002932549</v>
+      </c>
+      <c r="G56">
+        <f t="shared" si="1"/>
+        <v>2180.4194581535257</v>
+      </c>
+      <c r="J56">
+        <f t="shared" si="2"/>
+        <v>218.04194581535256</v>
+      </c>
+      <c r="K56">
+        <f t="shared" si="3"/>
+        <v>2180</v>
+      </c>
+    </row>
+    <row r="57" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E57">
+        <v>880</v>
+      </c>
+      <c r="F57" s="8">
+        <f t="shared" si="0"/>
+        <v>4.301075268817204</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="1"/>
+        <v>2222.805023749162</v>
+      </c>
+      <c r="J57">
+        <f t="shared" si="2"/>
+        <v>222.28050237491621</v>
+      </c>
+      <c r="K57">
+        <f t="shared" si="3"/>
+        <v>2222</v>
+      </c>
+    </row>
+    <row r="58" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E58">
+        <v>896</v>
+      </c>
+      <c r="F58" s="8">
+        <f t="shared" si="0"/>
+        <v>4.3792766373411531</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="1"/>
+        <v>2265.1905893447984</v>
+      </c>
+      <c r="J58">
+        <f t="shared" si="2"/>
+        <v>226.51905893447986</v>
+      </c>
+      <c r="K58">
+        <f t="shared" si="3"/>
+        <v>2265</v>
+      </c>
+    </row>
+    <row r="59" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E59">
+        <v>912</v>
+      </c>
+      <c r="F59" s="8">
+        <f t="shared" si="0"/>
+        <v>4.4574780058651022</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="1"/>
+        <v>2307.5761549404347</v>
+      </c>
+      <c r="J59">
+        <f t="shared" si="2"/>
+        <v>230.75761549404351</v>
+      </c>
+      <c r="K59">
+        <f t="shared" si="3"/>
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="60" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E60">
+        <v>928</v>
+      </c>
+      <c r="F60" s="8">
+        <f t="shared" si="0"/>
+        <v>4.5356793743890522</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="1"/>
+        <v>2349.9617205360714</v>
+      </c>
+      <c r="J60">
+        <f t="shared" si="2"/>
+        <v>234.99617205360715</v>
+      </c>
+      <c r="K60">
+        <f t="shared" si="3"/>
+        <v>2349</v>
+      </c>
+    </row>
+    <row r="61" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E61">
+        <v>944</v>
+      </c>
+      <c r="F61" s="8">
+        <f t="shared" si="0"/>
+        <v>4.6138807429130013</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="1"/>
+        <v>2392.3472861317077</v>
+      </c>
+      <c r="J61">
+        <f t="shared" si="2"/>
+        <v>239.23472861317077</v>
+      </c>
+      <c r="K61">
+        <f t="shared" si="3"/>
+        <v>2392</v>
+      </c>
+    </row>
+    <row r="62" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E62">
+        <v>960</v>
+      </c>
+      <c r="F62" s="8">
+        <f t="shared" si="0"/>
+        <v>4.6920821114369504</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="1"/>
+        <v>2434.732851727344</v>
+      </c>
+      <c r="J62">
+        <f t="shared" si="2"/>
+        <v>243.47328517273442</v>
+      </c>
+      <c r="K62">
+        <f t="shared" si="3"/>
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="63" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E63">
+        <v>976</v>
+      </c>
+      <c r="F63" s="8">
+        <f t="shared" si="0"/>
+        <v>4.7702834799608995</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="1"/>
+        <v>2477.1184173229808</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="2"/>
+        <v>247.71184173229807</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="3"/>
+        <v>2476</v>
+      </c>
+    </row>
+    <row r="64" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E64">
+        <v>992</v>
+      </c>
+      <c r="F64" s="8">
+        <f t="shared" si="0"/>
+        <v>4.8484848484848486</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="1"/>
+        <v>2519.5039829186171</v>
+      </c>
+      <c r="J64">
+        <f t="shared" si="2"/>
+        <v>251.95039829186169</v>
+      </c>
+      <c r="K64">
+        <f t="shared" si="3"/>
+        <v>2519</v>
+      </c>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E65">
+        <v>1008</v>
+      </c>
+      <c r="F65" s="8">
+        <f t="shared" si="0"/>
+        <v>4.9266862170087977</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="1"/>
+        <v>2561.8895485142534</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="2"/>
+        <v>256.18895485142536</v>
+      </c>
+      <c r="K65">
+        <f t="shared" si="3"/>
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="66" spans="5:11" x14ac:dyDescent="0.2">
+      <c r="E66">
+        <v>1024</v>
+      </c>
+      <c r="F66" s="8">
+        <f t="shared" si="0"/>
+        <v>5.0048875855327468</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="1"/>
+        <v>2604.2751141098897</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="2"/>
+        <v>260.42751141098898</v>
+      </c>
+      <c r="K66">
+        <f t="shared" si="3"/>
+        <v>2604</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>